<commit_message>
Modification fonction de base
Ajout des équations de modification du modèle à la fonction de base (sur un nouveau script).
</commit_message>
<xml_diff>
--- a/RENOMMAGE_PARAMETRES.xlsx
+++ b/RENOMMAGE_PARAMETRES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p_a_8\Documents\GitHub\MEPI-Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bclem\OneDrive\Documents\GitHub\MEPI-Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368ECFC1-EE24-4E5A-8F93-3C4FF9653038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A17BBC-06AD-4BD9-811C-D2DE43E130C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>l comme loss</t>
   </si>
   <si>
-    <t>taux mortalité P</t>
-  </si>
-  <si>
     <t>m_J</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>b_1</t>
   </si>
   <si>
-    <t>mortalité lié à infection par environnement</t>
-  </si>
-  <si>
     <t>b_2</t>
   </si>
   <si>
@@ -159,22 +153,28 @@
     <t>α_A</t>
   </si>
   <si>
-    <t>proportion d'interaction avec l'environnement infectieux de la classe L</t>
-  </si>
-  <si>
-    <t>proportion d'interaction avec l'environnement infectieux de la classe J</t>
-  </si>
-  <si>
-    <t>proportion d'interaction avec l'environnement infectieux de la classe A</t>
-  </si>
-  <si>
-    <t>taux de diffusion du pathogène par classe L</t>
-  </si>
-  <si>
-    <t>taux de diffusion du pathogène par classe J</t>
-  </si>
-  <si>
-    <t>taux de diffusion du pathogène par classe A</t>
+    <t>taux de diffusion du pathogène par classe L (eta1)</t>
+  </si>
+  <si>
+    <t>taux de diffusion du pathogène par classe J (eta2)</t>
+  </si>
+  <si>
+    <t>taux de diffusion du pathogène par classe A (eta3)</t>
+  </si>
+  <si>
+    <t>taux mortalité P (mpath)</t>
+  </si>
+  <si>
+    <t>Taux d'infection par les pathogènes libres (trans2)</t>
+  </si>
+  <si>
+    <t>proportion d'interaction avec l'environnement infectieux de la classe L (a1)</t>
+  </si>
+  <si>
+    <t>proportion d'interaction avec l'environnement infectieux de la classe J (a2)</t>
+  </si>
+  <si>
+    <t>proportion d'interaction avec l'environnement infectieux de la classe A (a3)</t>
   </si>
 </sst>
 </file>
@@ -265,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,9 +286,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,17 +636,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +655,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -667,7 +664,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -676,52 +673,52 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -732,36 +729,36 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -772,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -783,7 +780,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -794,7 +791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -805,86 +802,86 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>18</v>

</xml_diff>